<commit_message>
update kelp counts curation so worksheets are named (by site)
</commit_message>
<xml_diff>
--- a/curation/kelp_counts_curated.xlsx
+++ b/curation/kelp_counts_curated.xlsx
@@ -7,17 +7,17 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
-    <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
+    <sheet name="abur" sheetId="1" r:id="rId1"/>
+    <sheet name="ahnd" sheetId="2" r:id="rId2"/>
+    <sheet name="aque" sheetId="3" r:id="rId3"/>
+    <sheet name="bull" sheetId="4" r:id="rId4"/>
+    <sheet name="carp" sheetId="5" r:id="rId5"/>
+    <sheet name="golb" sheetId="6" r:id="rId6"/>
+    <sheet name="ivee" sheetId="7" r:id="rId7"/>
+    <sheet name="mohk" sheetId="8" r:id="rId8"/>
+    <sheet name="napl" sheetId="9" r:id="rId9"/>
+    <sheet name="scdi" sheetId="10" r:id="rId10"/>
+    <sheet name="sctw" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>

<commit_message>
update kelp curation (-common_name)
</commit_message>
<xml_diff>
--- a/curation/kelp_counts_curated.xlsx
+++ b/curation/kelp_counts_curated.xlsx
@@ -361,7 +361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -385,11 +385,6 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>common_name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>tot_fronds</t>
         </is>
       </c>
@@ -410,12 +405,7 @@
           <t>abur</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <v>307</v>
       </c>
     </row>
@@ -435,12 +425,7 @@
           <t>abur</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E3">
+      <c r="D3">
         <v>604</v>
       </c>
     </row>
@@ -460,12 +445,7 @@
           <t>abur</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E4">
+      <c r="D4">
         <v>3532</v>
       </c>
     </row>
@@ -476,7 +456,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -500,11 +480,6 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>common_name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>tot_fronds</t>
         </is>
       </c>
@@ -525,12 +500,7 @@
           <t>scdi</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <v>16</v>
       </c>
     </row>
@@ -550,12 +520,7 @@
           <t>scdi</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E3">
+      <c r="D3">
         <v>16</v>
       </c>
     </row>
@@ -575,12 +540,7 @@
           <t>scdi</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E4">
+      <c r="D4">
         <v>16</v>
       </c>
     </row>
@@ -591,7 +551,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -615,11 +575,6 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>common_name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>tot_fronds</t>
         </is>
       </c>
@@ -640,12 +595,7 @@
           <t>sctw</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <v>712</v>
       </c>
     </row>
@@ -665,12 +615,7 @@
           <t>sctw</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E3">
+      <c r="D3">
         <v>17</v>
       </c>
     </row>
@@ -690,12 +635,7 @@
           <t>sctw</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E4">
+      <c r="D4">
         <v>16</v>
       </c>
     </row>
@@ -706,7 +646,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -730,11 +670,6 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>common_name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>tot_fronds</t>
         </is>
       </c>
@@ -755,12 +690,7 @@
           <t>ahnd</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <v>2572</v>
       </c>
     </row>
@@ -780,12 +710,7 @@
           <t>ahnd</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E3">
+      <c r="D3">
         <v>16</v>
       </c>
     </row>
@@ -805,12 +730,7 @@
           <t>ahnd</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E4">
+      <c r="D4">
         <v>16</v>
       </c>
     </row>
@@ -821,7 +741,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -845,11 +765,6 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>common_name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>tot_fronds</t>
         </is>
       </c>
@@ -870,12 +785,7 @@
           <t>aque</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <v>11152</v>
       </c>
     </row>
@@ -895,12 +805,7 @@
           <t>aque</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E3">
+      <c r="D3">
         <v>9194</v>
       </c>
     </row>
@@ -920,12 +825,7 @@
           <t>aque</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E4">
+      <c r="D4">
         <v>7754</v>
       </c>
     </row>
@@ -936,7 +836,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -960,11 +860,6 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>common_name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>tot_fronds</t>
         </is>
       </c>
@@ -985,12 +880,7 @@
           <t>bull</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <v>6706</v>
       </c>
     </row>
@@ -1010,12 +900,7 @@
           <t>bull</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E3">
+      <c r="D3">
         <v>2505</v>
       </c>
     </row>
@@ -1026,7 +911,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1050,11 +935,6 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>common_name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>tot_fronds</t>
         </is>
       </c>
@@ -1075,12 +955,7 @@
           <t>carp</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <v>105504</v>
       </c>
     </row>
@@ -1100,12 +975,7 @@
           <t>carp</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E3">
+      <c r="D3">
         <v>47466</v>
       </c>
     </row>
@@ -1125,12 +995,7 @@
           <t>carp</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E4">
+      <c r="D4">
         <v>5477</v>
       </c>
     </row>
@@ -1141,7 +1006,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1165,11 +1030,6 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>common_name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>tot_fronds</t>
         </is>
       </c>
@@ -1190,12 +1050,7 @@
           <t>golb</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <v>2557</v>
       </c>
     </row>
@@ -1215,12 +1070,7 @@
           <t>golb</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E3">
+      <c r="D3">
         <v>1575</v>
       </c>
     </row>
@@ -1240,12 +1090,7 @@
           <t>golb</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E4">
+      <c r="D4">
         <v>1629</v>
       </c>
     </row>
@@ -1256,7 +1101,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1280,11 +1125,6 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>common_name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>tot_fronds</t>
         </is>
       </c>
@@ -1305,12 +1145,7 @@
           <t>ivee</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <v>24994</v>
       </c>
     </row>
@@ -1330,12 +1165,7 @@
           <t>ivee</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E3">
+      <c r="D3">
         <v>13371</v>
       </c>
     </row>
@@ -1355,12 +1185,7 @@
           <t>ivee</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E4">
+      <c r="D4">
         <v>9051</v>
       </c>
     </row>
@@ -1371,7 +1196,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1395,11 +1220,6 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>common_name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>tot_fronds</t>
         </is>
       </c>
@@ -1420,12 +1240,7 @@
           <t>mohk</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <v>21444</v>
       </c>
     </row>
@@ -1445,12 +1260,7 @@
           <t>mohk</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E3">
+      <c r="D3">
         <v>6347</v>
       </c>
     </row>
@@ -1470,12 +1280,7 @@
           <t>mohk</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E4">
+      <c r="D4">
         <v>3946</v>
       </c>
     </row>
@@ -1486,7 +1291,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1510,11 +1315,6 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>common_name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>tot_fronds</t>
         </is>
       </c>
@@ -1535,12 +1335,7 @@
           <t>napl</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <v>63366</v>
       </c>
     </row>
@@ -1560,12 +1355,7 @@
           <t>napl</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E3">
+      <c r="D3">
         <v>91719</v>
       </c>
     </row>
@@ -1585,12 +1375,7 @@
           <t>napl</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>giant kelp</t>
-        </is>
-      </c>
-      <c r="E4">
+      <c r="D4">
         <v>20747</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated to total_fronds in kelp curation
</commit_message>
<xml_diff>
--- a/curation/kelp_counts_curated.xlsx
+++ b/curation/kelp_counts_curated.xlsx
@@ -385,7 +385,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tot_fronds</t>
+          <t>total_fronds</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tot_fronds</t>
+          <t>total_fronds</t>
         </is>
       </c>
     </row>
@@ -575,7 +575,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tot_fronds</t>
+          <t>total_fronds</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tot_fronds</t>
+          <t>total_fronds</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tot_fronds</t>
+          <t>total_fronds</t>
         </is>
       </c>
     </row>
@@ -860,7 +860,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tot_fronds</t>
+          <t>total_fronds</t>
         </is>
       </c>
     </row>
@@ -935,7 +935,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tot_fronds</t>
+          <t>total_fronds</t>
         </is>
       </c>
     </row>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tot_fronds</t>
+          <t>total_fronds</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tot_fronds</t>
+          <t>total_fronds</t>
         </is>
       </c>
     </row>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tot_fronds</t>
+          <t>total_fronds</t>
         </is>
       </c>
     </row>
@@ -1315,7 +1315,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tot_fronds</t>
+          <t>total_fronds</t>
         </is>
       </c>
     </row>

</xml_diff>